<commit_message>
Added code to firstly make Binaps tables usable TODO: merging code with Binaps partitions
</commit_message>
<xml_diff>
--- a/experimentalResults/Comparison-altogether-avgValues(Recuperado automáticamente).xlsx
+++ b/experimentalResults/Comparison-altogether-avgValues(Recuperado automáticamente).xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbobed\workingDir\git\PartMining\experimentalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A52A494-8165-4419-9D64-B7B3214054B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5C2269-7033-4F3D-B337-62027724BE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD3DFA2-78C8-458F-A4D4-44EB572CE8BE}"/>
+    <workbookView xWindow="-23235" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{7BD3DFA2-78C8-458F-A4D4-44EB572CE8BE}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6512,7 +6511,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -24825,8 +24823,8 @@
   <dimension ref="A1:L188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B106" sqref="B106:L106"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG92" sqref="AG92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>